<commit_message>
update tests and data xl files
</commit_message>
<xml_diff>
--- a/inst/OM.xlsx
+++ b/inst/OM.xlsx
@@ -264,12 +264,12 @@
     <t xml:space="preserve">Irefbiascv</t>
   </si>
   <si>
+    <t xml:space="preserve">Brefbiascv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crefbiascv</t>
   </si>
   <si>
-    <t xml:space="preserve">Brefbiascv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dbiascv</t>
   </si>
   <si>
@@ -282,22 +282,22 @@
     <t xml:space="preserve">Recbiascv</t>
   </si>
   <si>
+    <t xml:space="preserve">TACFrac</t>
+  </si>
+  <si>
     <t xml:space="preserve">TACSD</t>
   </si>
   <si>
-    <t xml:space="preserve">TACFrac</t>
+    <t xml:space="preserve">TAEFrac</t>
   </si>
   <si>
     <t xml:space="preserve">TAESD</t>
   </si>
   <si>
-    <t xml:space="preserve">TAEFrac</t>
+    <t xml:space="preserve">SizeLimFrac</t>
   </si>
   <si>
     <t xml:space="preserve">SizeLimSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SizeLimFrac</t>
   </si>
   <si>
     <t xml:space="preserve">Agency</t>
@@ -1233,11 +1233,6 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>